<commit_message>
detalle fornato resultados encuesta
</commit_message>
<xml_diff>
--- a/ActualizacionDocente/XLSX/plantillaIndicadoresEncuesta.xlsx
+++ b/ActualizacionDocente/XLSX/plantillaIndicadoresEncuesta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Residencia\ActualizacionDocente\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891E68F7-D37F-494B-9CBD-8172175F100E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A756A66E-B854-4984-890E-4BF08DDA3442}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0C8322C2-4061-4828-B4CE-DCAA2CEACEC9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20280" windowHeight="10920" xr2:uid="{0C8322C2-4061-4828-B4CE-DCAA2CEACEC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>INSTITUTO TECNOLÓGICO DE DURANGO</t>
   </si>
@@ -72,10 +72,13 @@
     <t>Resultados de Encuesta del Curso</t>
   </si>
   <si>
-    <t>Promedio</t>
-  </si>
-  <si>
     <t>Totales</t>
+  </si>
+  <si>
+    <t>Total de puntos</t>
+  </si>
+  <si>
+    <t>Promedio de puntos</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -341,11 +344,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -354,67 +368,80 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,384 +809,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989087CA-2E46-4869-A6DD-412CC81B694B}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="C8" sqref="C8:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="3" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="13" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>5</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>6</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>7</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>8</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>9</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>10</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>11</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>12</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>13</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>14</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>15</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>16</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>17</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>18</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>19</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>20</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="25"/>
-    </row>
-    <row r="41" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1175,12 +1229,12 @@
     <row r="61" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C10:H10"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B3:H5"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:I5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>